<commit_message>
Alpha v2.1 - File Template Excel updated
</commit_message>
<xml_diff>
--- a/TemplateFlightLog.xlsx
+++ b/TemplateFlightLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrealunaro/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrealunaro/Desktop/stampe e progetti/VFR Planner/web app/v 2.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690DF79B-9327-BD4F-B545-1E9C1D11F221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA34D4A-4D82-534E-B698-989E75EBAB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25580" yWindow="4920" windowWidth="34680" windowHeight="26020" xr2:uid="{5B27618F-093B-204F-BA36-DF89F4747C30}"/>
+    <workbookView xWindow="25480" yWindow="4920" windowWidth="34680" windowHeight="26020" xr2:uid="{5B27618F-093B-204F-BA36-DF89F4747C30}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Foglio1!$A$1:$S$26</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -747,6 +748,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,6 +829,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -770,87 +852,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,9 +871,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -910,7 +911,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1016,7 +1017,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1158,7 +1159,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1172,7 +1173,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21:P21"/>
+      <selection activeCell="O25" sqref="O25:P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,64 +1182,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="37"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="37"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="34"/>
     </row>
     <row r="2" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="40"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="40"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="37"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="40"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
@@ -1321,56 +1322,56 @@
       <c r="S7" s="46"/>
     </row>
     <row r="8" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="34"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="34"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="43"/>
     </row>
     <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26" t="s">
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-      <c r="K9" s="24" t="s">
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="K9" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="26" t="s">
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26" t="s">
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="R9" s="26"/>
-      <c r="S9" s="27"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="50"/>
     </row>
     <row r="10" spans="1:19" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1618,20 +1619,20 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="9"/>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="29"/>
-      <c r="O20" s="30" t="s">
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="30" t="s">
+      <c r="P20" s="58"/>
+      <c r="Q20" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="R20" s="31"/>
+      <c r="R20" s="58"/>
       <c r="S20" s="23" t="s">
         <v>14</v>
       </c>
@@ -1646,19 +1647,19 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="9"/>
-      <c r="K21" s="51" t="s">
+      <c r="K21" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="54"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="54">
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="27">
         <f>0.72*O21</f>
         <v>0</v>
       </c>
-      <c r="R21" s="55"/>
+      <c r="R21" s="28"/>
       <c r="S21" s="22">
         <f>2.2*Q21</f>
         <v>0</v>
@@ -1674,19 +1675,19 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="9"/>
-      <c r="K22" s="51" t="s">
+      <c r="K22" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="54"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="54">
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="27">
         <f t="shared" ref="Q22:Q26" si="0">0.72*O22</f>
         <v>0</v>
       </c>
-      <c r="R22" s="55"/>
+      <c r="R22" s="28"/>
       <c r="S22" s="22">
         <f t="shared" ref="S22:S26" si="1">2.2*Q22</f>
         <v>0</v>
@@ -1702,19 +1703,19 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="9"/>
-      <c r="K23" s="56" t="s">
+      <c r="K23" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="54">
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R23" s="55"/>
+      <c r="R23" s="28"/>
       <c r="S23" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1730,19 +1731,19 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="9"/>
-      <c r="K24" s="51" t="s">
+      <c r="K24" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="52"/>
-      <c r="M24" s="52"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="54">
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R24" s="55"/>
+      <c r="R24" s="28"/>
       <c r="S24" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1758,58 +1759,88 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="18"/>
-      <c r="K25" s="51" t="s">
+      <c r="K25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="52"/>
-      <c r="M25" s="52"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="54">
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R25" s="55"/>
+      <c r="R25" s="28"/>
       <c r="S25" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="K26" s="51" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="K26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="54">
-        <f>O25-SUM(O21:P24)</f>
-        <v>0</v>
-      </c>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="55"/>
-      <c r="S26" s="22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="1:19" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="K8:S8"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="K3:S3"/>
+    <mergeCell ref="K4:S4"/>
+    <mergeCell ref="K5:S5"/>
+    <mergeCell ref="K6:S6"/>
+    <mergeCell ref="K7:S7"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="O26:P26"/>
     <mergeCell ref="Q26:R26"/>
@@ -1826,45 +1857,6 @@
     <mergeCell ref="K21:N21"/>
     <mergeCell ref="K22:N22"/>
     <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K8:S8"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="K3:S3"/>
-    <mergeCell ref="K4:S4"/>
-    <mergeCell ref="K5:S5"/>
-    <mergeCell ref="K6:S6"/>
-    <mergeCell ref="K7:S7"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="59" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>